<commit_message>
Removed comments, laterality. Reworked alcohol usage archetype.
</commit_message>
<xml_diff>
--- a/data/Mapping mellom register og Datamart.xlsx
+++ b/data/Mapping mellom register og Datamart.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helsevest-my.sharepoint.com/personal/rttn_ihelse_net/Documents/0 Protonregister/6 Eksport fra DIPS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rttn\source\repos\ehr_xml\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="11_F377A19E80A7CFA0CCE33B717A141B7D5E734144" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61AFC919-1683-4B4A-871A-734DD8A764F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6BB209-DE9E-4B48-9348-AB474C597782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admission" sheetId="1" r:id="rId1"/>
     <sheet name="Evaluation" sheetId="2" r:id="rId2"/>
-    <sheet name="Mappet mot Register" sheetId="4" r:id="rId3"/>
+    <sheet name="Mappet mot Register Original" sheetId="4" r:id="rId3"/>
+    <sheet name="Mappet mot Justert Register" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Evaluation!$A$3:$H$190</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="713">
   <si>
     <t>Ordinal</t>
   </si>
@@ -1979,6 +1980,207 @@
   </si>
   <si>
     <t>Er bildediagnostiske undersøkelser gjennomført?</t>
+  </si>
+  <si>
+    <t>Hva er denne variabelen?</t>
+  </si>
+  <si>
+    <t>Er dette den menneskelige lesbare?</t>
+  </si>
+  <si>
+    <t>Anatomisk lokalisering (inkl. lateralitet)</t>
+  </si>
+  <si>
+    <t>Primærdiagnose</t>
+  </si>
+  <si>
+    <t>Primærdiagnose ICD10-kode</t>
+  </si>
+  <si>
+    <t>Primærdiagnose ICD10-term</t>
+  </si>
+  <si>
+    <t>Aktuell komorbiditet</t>
+  </si>
+  <si>
+    <t>Aktuell komorbiditet, kategori</t>
+  </si>
+  <si>
+    <t>Aktuell komorbiditet, kommentar</t>
+  </si>
+  <si>
+    <t>Aktuell komorbiditet ICD10-kode</t>
+  </si>
+  <si>
+    <t>Aktuell komorbiditet ICD10-term</t>
+  </si>
+  <si>
+    <t>Stråleterapi volumnavn</t>
+  </si>
+  <si>
+    <t>Stråleterapi planlagt dose [Gy]</t>
+  </si>
+  <si>
+    <t>Stråleterapi antall fraksjoner planlagt</t>
+  </si>
+  <si>
+    <t>Stråleterapi fraksjoner per uke planlagt</t>
+  </si>
+  <si>
+    <t>Stråleterapi fraksjonsdoser planlagt</t>
+  </si>
+  <si>
+    <t>Stråleterapi gitt dose [Gy]</t>
+  </si>
+  <si>
+    <t>Stråleterapi antall fraksjoner gitt</t>
+  </si>
+  <si>
+    <t>Stråleterapi fraksjoner per uke gitt</t>
+  </si>
+  <si>
+    <t>Stråleterapi fraksjonsdoser gitt</t>
+  </si>
+  <si>
+    <t>Senskade dato for registrering</t>
+  </si>
+  <si>
+    <t>Senskade overordnet kategori</t>
+  </si>
+  <si>
+    <t>Senskade navngivning</t>
+  </si>
+  <si>
+    <t>Senskade grad</t>
+  </si>
+  <si>
+    <t>Senskade kodeverk for navngivning, versjon</t>
+  </si>
+  <si>
+    <t>Senskade kodeverk for grad, versjon</t>
+  </si>
+  <si>
+    <t>Senskade kommentar</t>
+  </si>
+  <si>
+    <t>Progresjon dato</t>
+  </si>
+  <si>
+    <t>Progresjon eller residiv</t>
+  </si>
+  <si>
+    <t>Progresjon metode for identifikasjon</t>
+  </si>
+  <si>
+    <t>Progresjon plassering / utbredelse</t>
+  </si>
+  <si>
+    <t>Progresjon kommentar</t>
+  </si>
+  <si>
+    <t>Navn på klinisk studie</t>
+  </si>
+  <si>
+    <t>Kontaktperson klinisk studie</t>
+  </si>
+  <si>
+    <t>Kommentar klinisk studie</t>
+  </si>
+  <si>
+    <t>Informert bredt samtykke</t>
+  </si>
+  <si>
+    <t>Informert samtykke register</t>
+  </si>
+  <si>
+    <t>Progresjon;Residiv</t>
+  </si>
+  <si>
+    <t>Lokal progresjon;Regional progresjon;Fjernmetastase</t>
+  </si>
+  <si>
+    <t>Histologi;Radiologi;Klinikk;Biokjemisk;Ukjent</t>
+  </si>
+  <si>
+    <t>Histologisk/morfologisk celletype</t>
+  </si>
+  <si>
+    <t>Topografisk mapping</t>
+  </si>
+  <si>
+    <t>Aminosyreendringer</t>
+  </si>
+  <si>
+    <t>Kreftform</t>
+  </si>
+  <si>
+    <t>Plassering</t>
+  </si>
+  <si>
+    <t>Diagnoseår</t>
+  </si>
+  <si>
+    <t>Gitt strålebehandling</t>
+  </si>
+  <si>
+    <t>Biologisk prøve identifikasjon</t>
+  </si>
+  <si>
+    <t>Biologisk prøve dato</t>
+  </si>
+  <si>
+    <t>Biologisk prøve opphav</t>
+  </si>
+  <si>
+    <t>Biologisk prøve type</t>
+  </si>
+  <si>
+    <t>Biologisk prøve lokasjon</t>
+  </si>
+  <si>
+    <t>Biologisk prøve fraksjon tumorceller [%]</t>
+  </si>
+  <si>
+    <t>Biologisk prøve kommentar</t>
+  </si>
+  <si>
+    <t>Biomarkør navn</t>
+  </si>
+  <si>
+    <t>Biomarkør verdi</t>
+  </si>
+  <si>
+    <t>Biomarkør enhet</t>
+  </si>
+  <si>
+    <t>Biomarkør kommentar</t>
+  </si>
+  <si>
+    <t>Navn på legemiddel / virkestoff / kur</t>
+  </si>
+  <si>
+    <t>Behandlingskategori</t>
+  </si>
+  <si>
+    <t>Terapeutisk hensikt</t>
+  </si>
+  <si>
+    <t>Totalmengde i perioden</t>
+  </si>
+  <si>
+    <t>Totalmengde i perioden (enhet)</t>
+  </si>
+  <si>
+    <t>Startdato for bruk</t>
+  </si>
+  <si>
+    <t>Sluttdato for bruk</t>
+  </si>
+  <si>
+    <t>Beskrivelse / kommentar</t>
+  </si>
+  <si>
+    <t>CTCAE (0 -5)</t>
   </si>
 </sst>
 </file>
@@ -2057,7 +2259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2088,6 +2290,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2288,7 +2496,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
@@ -2371,12 +2579,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2442,6 +2644,95 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40 % – uthevingsfarge 5" xfId="4" builtinId="47"/>
@@ -5063,8 +5354,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5080,10 +5371,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>640</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>637</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -5129,7 +5420,7 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="51" t="s">
         <v>277</v>
       </c>
       <c r="F4" t="s">
@@ -5152,7 +5443,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="51" t="s">
         <v>278</v>
       </c>
       <c r="F5" t="s">
@@ -5175,7 +5466,7 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="51" t="s">
         <v>279</v>
       </c>
       <c r="F6" t="s">
@@ -5198,7 +5489,7 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="51" t="s">
         <v>280</v>
       </c>
       <c r="F7" t="s">
@@ -5218,7 +5509,7 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="51" t="s">
         <v>281</v>
       </c>
       <c r="F8" t="s">
@@ -5238,7 +5529,7 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="51" t="s">
         <v>282</v>
       </c>
       <c r="F9" t="s">
@@ -5258,7 +5549,7 @@
       <c r="D10" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="51" t="s">
         <v>283</v>
       </c>
       <c r="F10" t="s">
@@ -5278,7 +5569,7 @@
       <c r="D11" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="51" t="s">
         <v>284</v>
       </c>
       <c r="F11" t="s">
@@ -5298,7 +5589,7 @@
       <c r="D12" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="51" t="s">
         <v>285</v>
       </c>
       <c r="F12" t="s">
@@ -5318,7 +5609,7 @@
       <c r="D13" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="51" t="s">
         <v>286</v>
       </c>
       <c r="F13" t="s">
@@ -5338,7 +5629,7 @@
       <c r="D14" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="51" t="s">
         <v>287</v>
       </c>
       <c r="F14" t="s">
@@ -5358,7 +5649,7 @@
       <c r="D15" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="51" t="s">
         <v>288</v>
       </c>
       <c r="F15" t="s">
@@ -5424,7 +5715,7 @@
       <c r="D18" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="51" t="s">
         <v>291</v>
       </c>
       <c r="F18" t="s">
@@ -5447,7 +5738,7 @@
       <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="51" t="s">
         <v>292</v>
       </c>
       <c r="F19" t="s">
@@ -5470,7 +5761,7 @@
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="51" t="s">
         <v>293</v>
       </c>
       <c r="F20" t="s">
@@ -5493,7 +5784,7 @@
       <c r="D21" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="51" t="s">
         <v>294</v>
       </c>
       <c r="F21" t="s">
@@ -5516,7 +5807,7 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="53" t="s">
+      <c r="E22" s="51" t="s">
         <v>295</v>
       </c>
       <c r="F22" t="s">
@@ -5539,7 +5830,7 @@
       <c r="D23" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="53" t="s">
+      <c r="E23" s="51" t="s">
         <v>296</v>
       </c>
       <c r="F23" t="s">
@@ -5562,7 +5853,7 @@
       <c r="D24" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="E24" s="51" t="s">
         <v>297</v>
       </c>
       <c r="F24" t="s">
@@ -5585,7 +5876,7 @@
       <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="51" t="s">
         <v>298</v>
       </c>
       <c r="F25" t="s">
@@ -5608,7 +5899,7 @@
       <c r="D26" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="53" t="s">
+      <c r="E26" s="51" t="s">
         <v>299</v>
       </c>
       <c r="F26" t="s">
@@ -5631,7 +5922,7 @@
       <c r="D27" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="51" t="s">
         <v>300</v>
       </c>
       <c r="F27" t="s">
@@ -5654,7 +5945,7 @@
       <c r="D28" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="53" t="s">
+      <c r="E28" s="51" t="s">
         <v>301</v>
       </c>
       <c r="F28" t="s">
@@ -5677,7 +5968,7 @@
       <c r="D29" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="53" t="s">
+      <c r="E29" s="51" t="s">
         <v>302</v>
       </c>
       <c r="F29" t="s">
@@ -5700,7 +5991,7 @@
       <c r="D30" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="53" t="s">
+      <c r="E30" s="51" t="s">
         <v>303</v>
       </c>
       <c r="F30" t="s">
@@ -5723,7 +6014,7 @@
       <c r="D31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="53" t="s">
+      <c r="E31" s="51" t="s">
         <v>304</v>
       </c>
       <c r="F31" t="s">
@@ -5746,7 +6037,7 @@
       <c r="D32" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="51" t="s">
         <v>305</v>
       </c>
       <c r="F32" t="s">
@@ -5769,7 +6060,7 @@
       <c r="D33" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="53" t="s">
+      <c r="E33" s="51" t="s">
         <v>306</v>
       </c>
       <c r="F33" t="s">
@@ -5792,7 +6083,7 @@
       <c r="D34" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="53" t="s">
+      <c r="E34" s="51" t="s">
         <v>307</v>
       </c>
       <c r="F34" t="s">
@@ -5815,7 +6106,7 @@
       <c r="D35" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="53" t="s">
+      <c r="E35" s="51" t="s">
         <v>308</v>
       </c>
       <c r="F35" t="s">
@@ -5835,7 +6126,7 @@
       <c r="D36" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="53" t="s">
+      <c r="E36" s="51" t="s">
         <v>309</v>
       </c>
       <c r="F36" t="s">
@@ -5941,7 +6232,7 @@
       <c r="D41" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="3" t="s">
         <v>314</v>
       </c>
       <c r="F41" t="s">
@@ -6053,7 +6344,7 @@
       <c r="D46" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="53" t="s">
+      <c r="E46" s="51" t="s">
         <v>319</v>
       </c>
       <c r="F46" t="s">
@@ -6076,7 +6367,7 @@
       <c r="D47" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="53" t="s">
+      <c r="E47" s="51" t="s">
         <v>320</v>
       </c>
       <c r="F47" t="s">
@@ -6099,7 +6390,7 @@
       <c r="D48" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="53" t="s">
+      <c r="E48" s="51" t="s">
         <v>321</v>
       </c>
       <c r="F48" t="s">
@@ -6122,7 +6413,7 @@
       <c r="D49" t="s">
         <v>53</v>
       </c>
-      <c r="E49" s="53" t="s">
+      <c r="E49" s="51" t="s">
         <v>322</v>
       </c>
       <c r="F49" t="s">
@@ -6145,7 +6436,7 @@
       <c r="D50" t="s">
         <v>55</v>
       </c>
-      <c r="E50" s="53" t="s">
+      <c r="E50" s="51" t="s">
         <v>323</v>
       </c>
       <c r="F50" t="s">
@@ -6165,7 +6456,7 @@
       <c r="D51" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="53" t="s">
+      <c r="E51" s="51" t="s">
         <v>324</v>
       </c>
       <c r="F51" t="s">
@@ -6300,7 +6591,7 @@
       <c r="D57" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="53" t="s">
+      <c r="E57" s="51" t="s">
         <v>330</v>
       </c>
       <c r="F57" t="s">
@@ -6323,7 +6614,7 @@
       <c r="D58" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="53" t="s">
+      <c r="E58" s="51" t="s">
         <v>331</v>
       </c>
       <c r="F58" t="s">
@@ -6346,7 +6637,7 @@
       <c r="D59" t="s">
         <v>13</v>
       </c>
-      <c r="E59" s="53" t="s">
+      <c r="E59" s="51" t="s">
         <v>332</v>
       </c>
       <c r="F59" t="s">
@@ -6369,7 +6660,7 @@
       <c r="D60" t="s">
         <v>53</v>
       </c>
-      <c r="E60" s="53" t="s">
+      <c r="E60" s="51" t="s">
         <v>333</v>
       </c>
       <c r="F60" t="s">
@@ -6561,7 +6852,7 @@
       <c r="D69" t="s">
         <v>112</v>
       </c>
-      <c r="E69" s="54" t="s">
+      <c r="E69" s="52" t="s">
         <v>342</v>
       </c>
       <c r="F69" t="s">
@@ -6684,7 +6975,7 @@
       <c r="D75" t="s">
         <v>118</v>
       </c>
-      <c r="E75" s="54" t="s">
+      <c r="E75" s="52" t="s">
         <v>348</v>
       </c>
       <c r="F75" t="s">
@@ -6724,7 +7015,7 @@
       <c r="D77" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="53" t="s">
+      <c r="E77" s="51" t="s">
         <v>350</v>
       </c>
       <c r="F77" t="s">
@@ -6747,7 +7038,7 @@
       <c r="D78" t="s">
         <v>9</v>
       </c>
-      <c r="E78" s="53" t="s">
+      <c r="E78" s="51" t="s">
         <v>351</v>
       </c>
       <c r="F78" t="s">
@@ -6770,7 +7061,7 @@
       <c r="D79" t="s">
         <v>13</v>
       </c>
-      <c r="E79" s="53" t="s">
+      <c r="E79" s="51" t="s">
         <v>352</v>
       </c>
       <c r="F79" t="s">
@@ -6793,7 +7084,7 @@
       <c r="D80" t="s">
         <v>53</v>
       </c>
-      <c r="E80" s="53" t="s">
+      <c r="E80" s="51" t="s">
         <v>353</v>
       </c>
       <c r="F80" t="s">
@@ -6856,7 +7147,7 @@
       <c r="D83" t="s">
         <v>122</v>
       </c>
-      <c r="E83" s="53" t="s">
+      <c r="E83" s="51" t="s">
         <v>356</v>
       </c>
       <c r="F83" t="s">
@@ -6879,7 +7170,7 @@
       <c r="D84" t="s">
         <v>5</v>
       </c>
-      <c r="E84" s="53" t="s">
+      <c r="E84" s="51" t="s">
         <v>357</v>
       </c>
       <c r="F84" t="s">
@@ -6902,7 +7193,7 @@
       <c r="D85" t="s">
         <v>9</v>
       </c>
-      <c r="E85" s="53" t="s">
+      <c r="E85" s="51" t="s">
         <v>358</v>
       </c>
       <c r="F85" t="s">
@@ -6925,7 +7216,7 @@
       <c r="D86" t="s">
         <v>13</v>
       </c>
-      <c r="E86" s="53" t="s">
+      <c r="E86" s="51" t="s">
         <v>359</v>
       </c>
       <c r="F86" t="s">
@@ -6948,7 +7239,7 @@
       <c r="D87" t="s">
         <v>53</v>
       </c>
-      <c r="E87" s="53" t="s">
+      <c r="E87" s="51" t="s">
         <v>360</v>
       </c>
       <c r="F87" t="s">
@@ -6966,7 +7257,7 @@
         <v>124</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -6988,6 +7279,9 @@
       <c r="A89" t="s">
         <v>124</v>
       </c>
+      <c r="B89" s="3" t="s">
+        <v>647</v>
+      </c>
       <c r="C89">
         <v>5</v>
       </c>
@@ -7054,7 +7348,7 @@
       <c r="D92" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="53" t="s">
+      <c r="E92" s="51" t="s">
         <v>365</v>
       </c>
       <c r="F92" t="s">
@@ -7077,7 +7371,7 @@
       <c r="D93" t="s">
         <v>9</v>
       </c>
-      <c r="E93" s="53" t="s">
+      <c r="E93" s="51" t="s">
         <v>366</v>
       </c>
       <c r="F93" t="s">
@@ -7100,7 +7394,7 @@
       <c r="D94" t="s">
         <v>13</v>
       </c>
-      <c r="E94" s="53" t="s">
+      <c r="E94" s="51" t="s">
         <v>367</v>
       </c>
       <c r="F94" t="s">
@@ -7123,7 +7417,7 @@
       <c r="D95" t="s">
         <v>53</v>
       </c>
-      <c r="E95" s="53" t="s">
+      <c r="E95" s="51" t="s">
         <v>368</v>
       </c>
       <c r="F95" t="s">
@@ -7137,16 +7431,17 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C96">
+      <c r="B96" s="3"/>
+      <c r="C96" s="3">
         <v>4</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="3" t="s">
         <v>369</v>
       </c>
       <c r="F96" t="s">
@@ -7157,16 +7452,17 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C97">
+      <c r="B97" s="3"/>
+      <c r="C97" s="3">
         <v>5</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="3" t="s">
         <v>370</v>
       </c>
       <c r="F97" t="s">
@@ -7177,16 +7473,17 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C98">
+      <c r="B98" s="3"/>
+      <c r="C98" s="3">
         <v>6</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="3" t="s">
         <v>371</v>
       </c>
       <c r="F98" t="s">
@@ -7197,16 +7494,17 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C99">
+      <c r="B99" s="3"/>
+      <c r="C99" s="3">
         <v>7</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="3" t="s">
         <v>372</v>
       </c>
       <c r="F99" t="s">
@@ -7217,16 +7515,17 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C100">
+      <c r="B100" s="3"/>
+      <c r="C100" s="3">
         <v>8</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="3" t="s">
         <v>373</v>
       </c>
       <c r="F100" t="s">
@@ -7249,7 +7548,7 @@
       <c r="D101" t="s">
         <v>5</v>
       </c>
-      <c r="E101" s="53" t="s">
+      <c r="E101" s="51" t="s">
         <v>374</v>
       </c>
       <c r="F101" t="s">
@@ -7275,7 +7574,7 @@
       <c r="D102" t="s">
         <v>9</v>
       </c>
-      <c r="E102" s="53" t="s">
+      <c r="E102" s="51" t="s">
         <v>375</v>
       </c>
       <c r="F102" t="s">
@@ -7301,7 +7600,7 @@
       <c r="D103" t="s">
         <v>13</v>
       </c>
-      <c r="E103" s="53" t="s">
+      <c r="E103" s="51" t="s">
         <v>376</v>
       </c>
       <c r="F103" t="s">
@@ -7327,7 +7626,7 @@
       <c r="D104" t="s">
         <v>53</v>
       </c>
-      <c r="E104" s="53" t="s">
+      <c r="E104" s="51" t="s">
         <v>377</v>
       </c>
       <c r="F104" t="s">
@@ -7353,7 +7652,7 @@
       <c r="D105" t="s">
         <v>133</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="52" t="s">
         <v>378</v>
       </c>
       <c r="F105" t="s">
@@ -7376,7 +7675,7 @@
       <c r="D106" t="s">
         <v>55</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E106" s="52" t="s">
         <v>379</v>
       </c>
       <c r="F106" t="s">
@@ -7399,7 +7698,7 @@
       <c r="D107" t="s">
         <v>56</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="52" t="s">
         <v>380</v>
       </c>
       <c r="F107" t="s">
@@ -7422,7 +7721,7 @@
       <c r="D108" t="s">
         <v>134</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="52" t="s">
         <v>381</v>
       </c>
       <c r="F108" t="s">
@@ -7445,7 +7744,7 @@
       <c r="D109" t="s">
         <v>135</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="52" t="s">
         <v>382</v>
       </c>
       <c r="F109" t="s">
@@ -7468,7 +7767,7 @@
       <c r="D110" t="s">
         <v>136</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="52" t="s">
         <v>383</v>
       </c>
       <c r="F110" t="s">
@@ -7491,7 +7790,7 @@
       <c r="D111" t="s">
         <v>92</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="52" t="s">
         <v>384</v>
       </c>
       <c r="F111" t="s">
@@ -7514,7 +7813,7 @@
       <c r="D112" t="s">
         <v>93</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="52" t="s">
         <v>385</v>
       </c>
       <c r="F112" t="s">
@@ -7537,7 +7836,7 @@
       <c r="D113" t="s">
         <v>94</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="52" t="s">
         <v>386</v>
       </c>
       <c r="F113" t="s">
@@ -7560,7 +7859,7 @@
       <c r="D114" t="s">
         <v>5</v>
       </c>
-      <c r="E114" s="53" t="s">
+      <c r="E114" s="51" t="s">
         <v>387</v>
       </c>
       <c r="F114" t="s">
@@ -7586,7 +7885,7 @@
       <c r="D115" t="s">
         <v>9</v>
       </c>
-      <c r="E115" s="53" t="s">
+      <c r="E115" s="51" t="s">
         <v>388</v>
       </c>
       <c r="F115" t="s">
@@ -7612,7 +7911,7 @@
       <c r="D116" t="s">
         <v>13</v>
       </c>
-      <c r="E116" s="53" t="s">
+      <c r="E116" s="51" t="s">
         <v>389</v>
       </c>
       <c r="F116" t="s">
@@ -7638,7 +7937,7 @@
       <c r="D117" t="s">
         <v>53</v>
       </c>
-      <c r="E117" s="53" t="s">
+      <c r="E117" s="51" t="s">
         <v>390</v>
       </c>
       <c r="F117" t="s">
@@ -7664,7 +7963,7 @@
       <c r="D118" t="s">
         <v>133</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="52" t="s">
         <v>391</v>
       </c>
       <c r="F118" t="s">
@@ -7687,7 +7986,7 @@
       <c r="D119" t="s">
         <v>55</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="52" t="s">
         <v>392</v>
       </c>
       <c r="F119" t="s">
@@ -7710,7 +8009,7 @@
       <c r="D120" t="s">
         <v>56</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="52" t="s">
         <v>393</v>
       </c>
       <c r="F120" t="s">
@@ -7733,7 +8032,7 @@
       <c r="D121" t="s">
         <v>134</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="52" t="s">
         <v>394</v>
       </c>
       <c r="F121" t="s">
@@ -7756,7 +8055,7 @@
       <c r="D122" t="s">
         <v>138</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="52" t="s">
         <v>395</v>
       </c>
       <c r="F122" t="s">
@@ -7779,7 +8078,7 @@
       <c r="D123" t="s">
         <v>139</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="52" t="s">
         <v>396</v>
       </c>
       <c r="F123" t="s">
@@ -7799,7 +8098,7 @@
       <c r="D124" t="s">
         <v>5</v>
       </c>
-      <c r="E124" s="53" t="s">
+      <c r="E124" s="51" t="s">
         <v>397</v>
       </c>
       <c r="F124" t="s">
@@ -7822,7 +8121,7 @@
       <c r="D125" t="s">
         <v>9</v>
       </c>
-      <c r="E125" s="53" t="s">
+      <c r="E125" s="51" t="s">
         <v>398</v>
       </c>
       <c r="F125" t="s">
@@ -7845,7 +8144,7 @@
       <c r="D126" t="s">
         <v>13</v>
       </c>
-      <c r="E126" s="53" t="s">
+      <c r="E126" s="51" t="s">
         <v>399</v>
       </c>
       <c r="F126" t="s">
@@ -7868,7 +8167,7 @@
       <c r="D127" t="s">
         <v>53</v>
       </c>
-      <c r="E127" s="53" t="s">
+      <c r="E127" s="51" t="s">
         <v>400</v>
       </c>
       <c r="F127" t="s">
@@ -8029,7 +8328,7 @@
       <c r="D134" t="s">
         <v>56</v>
       </c>
-      <c r="E134" s="53" t="s">
+      <c r="E134" s="51" t="s">
         <v>407</v>
       </c>
       <c r="F134" t="s">
@@ -8049,7 +8348,7 @@
       <c r="D135" t="s">
         <v>55</v>
       </c>
-      <c r="E135" s="53" t="s">
+      <c r="E135" s="51" t="s">
         <v>408</v>
       </c>
       <c r="F135" t="s">
@@ -8069,7 +8368,7 @@
       <c r="D136" t="s">
         <v>5</v>
       </c>
-      <c r="E136" s="53" t="s">
+      <c r="E136" s="51" t="s">
         <v>409</v>
       </c>
       <c r="F136" t="s">
@@ -8092,7 +8391,7 @@
       <c r="D137" t="s">
         <v>9</v>
       </c>
-      <c r="E137" s="53" t="s">
+      <c r="E137" s="51" t="s">
         <v>410</v>
       </c>
       <c r="F137" t="s">
@@ -8115,7 +8414,7 @@
       <c r="D138" t="s">
         <v>13</v>
       </c>
-      <c r="E138" s="53" t="s">
+      <c r="E138" s="51" t="s">
         <v>411</v>
       </c>
       <c r="F138" t="s">
@@ -8138,7 +8437,7 @@
       <c r="D139" t="s">
         <v>53</v>
       </c>
-      <c r="E139" s="53" t="s">
+      <c r="E139" s="51" t="s">
         <v>412</v>
       </c>
       <c r="F139" t="s">
@@ -8161,7 +8460,7 @@
       <c r="D140" t="s">
         <v>55</v>
       </c>
-      <c r="E140" s="53" t="s">
+      <c r="E140" s="51" t="s">
         <v>413</v>
       </c>
       <c r="F140" t="s">
@@ -8267,7 +8566,7 @@
       <c r="D145" t="s">
         <v>5</v>
       </c>
-      <c r="E145" s="53" t="s">
+      <c r="E145" s="51" t="s">
         <v>418</v>
       </c>
       <c r="F145" t="s">
@@ -8290,7 +8589,7 @@
       <c r="D146" t="s">
         <v>9</v>
       </c>
-      <c r="E146" s="53" t="s">
+      <c r="E146" s="51" t="s">
         <v>419</v>
       </c>
       <c r="F146" t="s">
@@ -8313,7 +8612,7 @@
       <c r="D147" t="s">
         <v>13</v>
       </c>
-      <c r="E147" s="53" t="s">
+      <c r="E147" s="51" t="s">
         <v>420</v>
       </c>
       <c r="F147" t="s">
@@ -8336,7 +8635,7 @@
       <c r="D148" t="s">
         <v>53</v>
       </c>
-      <c r="E148" s="53" t="s">
+      <c r="E148" s="51" t="s">
         <v>421</v>
       </c>
       <c r="F148" t="s">
@@ -8359,7 +8658,7 @@
       <c r="D149" t="s">
         <v>55</v>
       </c>
-      <c r="E149" s="53" t="s">
+      <c r="E149" s="51" t="s">
         <v>422</v>
       </c>
       <c r="F149" t="s">
@@ -8511,7 +8810,7 @@
       <c r="D156" t="s">
         <v>56</v>
       </c>
-      <c r="E156" s="54" t="s">
+      <c r="E156" s="52" t="s">
         <v>429</v>
       </c>
       <c r="F156" t="s">
@@ -8531,7 +8830,7 @@
       <c r="D157" t="s">
         <v>152</v>
       </c>
-      <c r="E157" s="54" t="s">
+      <c r="E157" s="52" t="s">
         <v>430</v>
       </c>
       <c r="F157" t="s">
@@ -8551,7 +8850,7 @@
       <c r="D158" t="s">
         <v>153</v>
       </c>
-      <c r="E158" s="54" t="s">
+      <c r="E158" s="52" t="s">
         <v>431</v>
       </c>
       <c r="F158" t="s">
@@ -8571,7 +8870,7 @@
       <c r="D159" t="s">
         <v>154</v>
       </c>
-      <c r="E159" s="54" t="s">
+      <c r="E159" s="52" t="s">
         <v>432</v>
       </c>
       <c r="F159" t="s">
@@ -8683,7 +8982,7 @@
       <c r="D164" t="s">
         <v>56</v>
       </c>
-      <c r="E164" s="54" t="s">
+      <c r="E164" s="52" t="s">
         <v>437</v>
       </c>
       <c r="F164" t="s">
@@ -8703,7 +9002,7 @@
       <c r="D165" t="s">
         <v>156</v>
       </c>
-      <c r="E165" s="54" t="s">
+      <c r="E165" s="52" t="s">
         <v>438</v>
       </c>
       <c r="F165" t="s">
@@ -8723,7 +9022,7 @@
       <c r="D166" t="s">
         <v>157</v>
       </c>
-      <c r="E166" s="54" t="s">
+      <c r="E166" s="52" t="s">
         <v>439</v>
       </c>
       <c r="F166" t="s">
@@ -8743,7 +9042,7 @@
       <c r="D167" t="s">
         <v>158</v>
       </c>
-      <c r="E167" s="54" t="s">
+      <c r="E167" s="52" t="s">
         <v>440</v>
       </c>
       <c r="F167" t="s">
@@ -8855,7 +9154,7 @@
       <c r="D172" t="s">
         <v>161</v>
       </c>
-      <c r="E172" s="54" t="s">
+      <c r="E172" s="52" t="s">
         <v>445</v>
       </c>
       <c r="F172" t="s">
@@ -8875,7 +9174,7 @@
       <c r="D173" t="s">
         <v>162</v>
       </c>
-      <c r="E173" s="54" t="s">
+      <c r="E173" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F173" t="s">
@@ -8895,7 +9194,7 @@
       <c r="D174" t="s">
         <v>163</v>
       </c>
-      <c r="E174" s="54" t="s">
+      <c r="E174" s="52" t="s">
         <v>447</v>
       </c>
       <c r="F174" t="s">
@@ -8915,7 +9214,7 @@
       <c r="D175" t="s">
         <v>164</v>
       </c>
-      <c r="E175" s="54" t="s">
+      <c r="E175" s="52" t="s">
         <v>448</v>
       </c>
       <c r="F175" t="s">
@@ -8935,7 +9234,7 @@
       <c r="D176" t="s">
         <v>165</v>
       </c>
-      <c r="E176" s="54" t="s">
+      <c r="E176" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F176" t="s">
@@ -8955,7 +9254,7 @@
       <c r="D177" t="s">
         <v>166</v>
       </c>
-      <c r="E177" s="54" t="s">
+      <c r="E177" s="52" t="s">
         <v>450</v>
       </c>
       <c r="F177" t="s">
@@ -8975,7 +9274,7 @@
       <c r="D178" t="s">
         <v>167</v>
       </c>
-      <c r="E178" s="54" t="s">
+      <c r="E178" s="52" t="s">
         <v>451</v>
       </c>
       <c r="F178" t="s">
@@ -8995,7 +9294,7 @@
       <c r="D179" t="s">
         <v>168</v>
       </c>
-      <c r="E179" s="54" t="s">
+      <c r="E179" s="52" t="s">
         <v>452</v>
       </c>
       <c r="F179" t="s">
@@ -9015,7 +9314,7 @@
       <c r="D180" t="s">
         <v>169</v>
       </c>
-      <c r="E180" s="54" t="s">
+      <c r="E180" s="52" t="s">
         <v>453</v>
       </c>
       <c r="F180" t="s">
@@ -9132,7 +9431,7 @@
       <c r="D185" t="s">
         <v>81</v>
       </c>
-      <c r="E185" s="54" t="s">
+      <c r="E185" s="52" t="s">
         <v>458</v>
       </c>
       <c r="F185" t="s">
@@ -9153,7 +9452,7 @@
       <c r="D186" t="s">
         <v>170</v>
       </c>
-      <c r="E186" s="54" t="s">
+      <c r="E186" s="52" t="s">
         <v>459</v>
       </c>
       <c r="F186" t="s">
@@ -9174,7 +9473,7 @@
       <c r="D187" t="s">
         <v>171</v>
       </c>
-      <c r="E187" s="54" t="s">
+      <c r="E187" s="52" t="s">
         <v>460</v>
       </c>
       <c r="F187" t="s">
@@ -9195,7 +9494,7 @@
       <c r="D188" t="s">
         <v>164</v>
       </c>
-      <c r="E188" s="54" t="s">
+      <c r="E188" s="52" t="s">
         <v>461</v>
       </c>
       <c r="F188" t="s">
@@ -9286,11 +9585,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645DA601-D7B8-4DD6-8072-D92BB6C7F4C2}">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9623,541 +9922,1468 @@
       </c>
       <c r="B39" s="15"/>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
-        <v>526</v>
-      </c>
-      <c r="B40" s="31" t="s">
+    <row r="40" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="B40" s="29" t="s">
         <v>527</v>
       </c>
       <c r="C40" t="s">
-        <v>528</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>529</v>
-      </c>
-      <c r="B41" s="29" t="s">
+      <c r="A41" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>500</v>
+      </c>
+      <c r="C41" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>535</v>
+      </c>
+      <c r="B44" s="32"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>536</v>
+      </c>
+      <c r="B45" s="34" t="s">
         <v>527</v>
       </c>
-      <c r="C41" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>530</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>500</v>
-      </c>
-      <c r="C42" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
-        <v>531</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
-        <v>533</v>
-      </c>
-      <c r="B44" s="27" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>535</v>
-      </c>
-      <c r="B45" s="34"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>527</v>
+        <v>500</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
-        <v>537</v>
-      </c>
-      <c r="B47" s="38" t="s">
-        <v>500</v>
+      <c r="A47" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
-        <v>538</v>
-      </c>
-      <c r="B48" s="38" t="s">
-        <v>539</v>
-      </c>
+      <c r="A48" s="35" t="s">
+        <v>540</v>
+      </c>
+      <c r="B48" s="36"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="s">
-        <v>540</v>
-      </c>
-      <c r="B49" s="38"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
         <v>541</v>
       </c>
-      <c r="B50" s="40" t="s">
+      <c r="B49" s="38" t="s">
         <v>527</v>
       </c>
     </row>
+    <row r="50" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>543</v>
+      </c>
+    </row>
     <row r="51" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>542</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>543</v>
+      <c r="A51" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="B51" s="39" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="B52" s="41" t="s">
-        <v>545</v>
+      <c r="A52" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>546</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>547</v>
+      <c r="A53" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="B53" s="40"/>
+      <c r="C53" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
-        <v>548</v>
-      </c>
-      <c r="B54" s="42"/>
+      <c r="A54" s="20" t="s">
+        <v>549</v>
+      </c>
+      <c r="B54" s="21"/>
       <c r="C54" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>549</v>
-      </c>
-      <c r="B55" s="21"/>
+        <v>550</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>551</v>
+      </c>
       <c r="C55" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>551</v>
-      </c>
-      <c r="C56" t="s">
-        <v>310</v>
+        <v>553</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>553</v>
+        <v>539</v>
+      </c>
+      <c r="C57" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B58" s="21" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="B59" s="23"/>
+    </row>
+    <row r="60" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="B60" s="25"/>
+      <c r="C60" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>559</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
+        <v>560</v>
+      </c>
+      <c r="B62" s="21"/>
+    </row>
+    <row r="63" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>561</v>
+      </c>
+      <c r="B63" s="21"/>
+      <c r="C63" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="B64" s="21"/>
+      <c r="C64" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
+        <v>563</v>
+      </c>
+      <c r="B65" s="21"/>
+      <c r="C65" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="B66" s="23"/>
+    </row>
+    <row r="67" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
+        <v>565</v>
+      </c>
+      <c r="B67" s="40"/>
+    </row>
+    <row r="68" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
+        <v>566</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="41" t="s">
+        <v>568</v>
+      </c>
+      <c r="B69" s="42" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
+        <v>570</v>
+      </c>
+      <c r="B70" s="21"/>
+    </row>
+    <row r="71" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="20" t="s">
+        <v>571</v>
+      </c>
+      <c r="B71" s="21"/>
+    </row>
+    <row r="72" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="20" t="s">
+        <v>572</v>
+      </c>
+      <c r="B72" s="21"/>
+    </row>
+    <row r="73" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="20" t="s">
+        <v>573</v>
+      </c>
+      <c r="B73" s="21"/>
+    </row>
+    <row r="74" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="B74" s="23"/>
+    </row>
+    <row r="75" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="B75" s="29" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="B76" s="15"/>
+    </row>
+    <row r="77" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="B77" s="15"/>
+    </row>
+    <row r="78" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="43" t="s">
+        <v>585</v>
+      </c>
+      <c r="B82" s="32"/>
+    </row>
+    <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="24" t="s">
+        <v>586</v>
+      </c>
+      <c r="B83" s="29"/>
+    </row>
+    <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="B84" s="15"/>
+    </row>
+    <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="B85" s="15"/>
+    </row>
+    <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="B86" s="44"/>
+    </row>
+    <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="B87" s="15"/>
+    </row>
+    <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="20" t="s">
+        <v>591</v>
+      </c>
+      <c r="B88" s="15"/>
+    </row>
+    <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="B89" s="15"/>
+    </row>
+    <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="B90" s="44"/>
+    </row>
+    <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="B91" s="29" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="B93" s="17"/>
+    </row>
+    <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="41" t="s">
+        <v>599</v>
+      </c>
+      <c r="B94" s="42" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="41" t="s">
+        <v>601</v>
+      </c>
+      <c r="B95" s="42" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="B96" s="42" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="41" t="s">
+        <v>605</v>
+      </c>
+      <c r="B97" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="41" t="s">
+        <v>607</v>
+      </c>
+      <c r="B98" s="42"/>
+    </row>
+    <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="41" t="s">
+        <v>608</v>
+      </c>
+      <c r="B99" s="42"/>
+    </row>
+    <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="45" t="s">
+        <v>609</v>
+      </c>
+      <c r="B100" s="46"/>
+    </row>
+    <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="28" t="s">
+        <v>610</v>
+      </c>
+      <c r="B101" s="29"/>
+    </row>
+    <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="14" t="s">
+        <v>611</v>
+      </c>
+      <c r="B102" s="15"/>
+    </row>
+    <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="B104" s="47"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="48" t="s">
+        <v>615</v>
+      </c>
+      <c r="B105" s="39" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="20" t="s">
+        <v>617</v>
+      </c>
+      <c r="B106" s="49" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="20" t="s">
+        <v>619</v>
+      </c>
+      <c r="B107" s="49" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="B108" s="50"/>
+    </row>
+    <row r="109" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="14" t="s">
+        <v>622</v>
+      </c>
+      <c r="B109" s="26" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="B110" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFAC4D6-AB08-414B-9094-D10AD21A1CBA}">
+  <dimension ref="A1:C119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="B4" s="13"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
+        <v>474</v>
+      </c>
+      <c r="B6" s="71"/>
+      <c r="C6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="70" t="s">
+        <v>475</v>
+      </c>
+      <c r="B7" s="71"/>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="70" t="s">
+        <v>476</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>477</v>
+      </c>
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="70" t="s">
+        <v>478</v>
+      </c>
+      <c r="B9" s="71"/>
+      <c r="C9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="70" t="s">
+        <v>479</v>
+      </c>
+      <c r="B10" s="71"/>
+      <c r="C10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="68" t="s">
+        <v>480</v>
+      </c>
+      <c r="B11" s="69"/>
+      <c r="C11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="98" t="s">
+        <v>493</v>
+      </c>
+      <c r="B19" s="99"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="59" t="s">
+        <v>494</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66" t="s">
+        <v>496</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>497</v>
+      </c>
+      <c r="C21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="68" t="s">
+        <v>498</v>
+      </c>
+      <c r="B22" s="69"/>
+      <c r="C22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>652</v>
+      </c>
+      <c r="B23" s="61" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58" t="s">
+        <v>655</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
+        <v>656</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="62" t="s">
+        <v>653</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="90" t="s">
+        <v>654</v>
+      </c>
+      <c r="B27" s="91"/>
+    </row>
+    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>649</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>500</v>
+      </c>
+      <c r="C28" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
+        <v>650</v>
+      </c>
+      <c r="B29" s="72" t="s">
+        <v>500</v>
+      </c>
+      <c r="C29"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>651</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>500</v>
+      </c>
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="53" t="s">
+        <v>506</v>
+      </c>
+      <c r="B31" s="54"/>
+    </row>
+    <row r="32" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>648</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="C34" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="90" t="s">
+        <v>511</v>
+      </c>
+      <c r="B35" s="91"/>
+    </row>
+    <row r="36" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>512</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>521</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="62" t="s">
+        <v>523</v>
+      </c>
+      <c r="B41" s="63"/>
+    </row>
+    <row r="42" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="62" t="s">
+        <v>524</v>
+      </c>
+      <c r="B42" s="63"/>
+    </row>
+    <row r="43" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="62" t="s">
+        <v>525</v>
+      </c>
+      <c r="B43" s="63"/>
+    </row>
+    <row r="44" spans="1:3" s="30" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="59" t="s">
+        <v>526</v>
+      </c>
+      <c r="B44" s="55" t="s">
+        <v>527</v>
+      </c>
+      <c r="C44" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>527</v>
+      </c>
+      <c r="C45" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>500</v>
+      </c>
+      <c r="C46" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="60" t="s">
+        <v>686</v>
+      </c>
+      <c r="B47" s="61" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="64" t="s">
+        <v>687</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="73" t="s">
+        <v>688</v>
+      </c>
+      <c r="B49" s="74"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="82" t="s">
+        <v>689</v>
+      </c>
+      <c r="B51" s="83" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="84" t="s">
+        <v>690</v>
+      </c>
+      <c r="B52" s="85" t="s">
         <v>539</v>
       </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="84" t="s">
+        <v>691</v>
+      </c>
+      <c r="B53" s="85"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="86" t="s">
+        <v>692</v>
+      </c>
+      <c r="B54" s="87" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="60" t="s">
+        <v>542</v>
+      </c>
+      <c r="B55" s="61" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="62" t="s">
+        <v>544</v>
+      </c>
+      <c r="B56" s="63" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="64" t="s">
+        <v>546</v>
+      </c>
+      <c r="B57" s="65" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>693</v>
+      </c>
+      <c r="B58" s="47"/>
       <c r="C58" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>555</v>
-      </c>
-      <c r="B59" s="21" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="B60" s="23"/>
+        <v>694</v>
+      </c>
+      <c r="B59" s="49"/>
+      <c r="C59" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="B60" s="49" t="s">
+        <v>551</v>
+      </c>
+      <c r="C60" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="61" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
-        <v>558</v>
-      </c>
-      <c r="B61" s="25"/>
-      <c r="C61" t="s">
-        <v>314</v>
+      <c r="A61" s="62" t="s">
+        <v>696</v>
+      </c>
+      <c r="B61" s="63" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>559</v>
-      </c>
-      <c r="B62" s="26"/>
+        <v>697</v>
+      </c>
+      <c r="B62" s="49" t="s">
+        <v>539</v>
+      </c>
       <c r="C62" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>560</v>
-      </c>
-      <c r="B63" s="21"/>
-    </row>
-    <row r="64" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
-        <v>561</v>
-      </c>
-      <c r="B64" s="21"/>
-      <c r="C64" t="s">
-        <v>316</v>
-      </c>
+      <c r="A63" s="62" t="s">
+        <v>698</v>
+      </c>
+      <c r="B63" s="63" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="88" t="s">
+        <v>699</v>
+      </c>
+      <c r="B64" s="89"/>
     </row>
     <row r="65" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
-        <v>562</v>
-      </c>
-      <c r="B65" s="21"/>
+      <c r="A65" s="24" t="s">
+        <v>700</v>
+      </c>
+      <c r="B65" s="29"/>
       <c r="C65" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>563</v>
-      </c>
-      <c r="B66" s="21"/>
+        <v>701</v>
+      </c>
+      <c r="B66" s="15"/>
       <c r="C66" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="B67" s="23"/>
+      <c r="A67" s="62" t="s">
+        <v>702</v>
+      </c>
+      <c r="B67" s="63"/>
     </row>
     <row r="68" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
-        <v>565</v>
-      </c>
-      <c r="B68" s="42"/>
+      <c r="A68" s="20" t="s">
+        <v>561</v>
+      </c>
+      <c r="B68" s="49"/>
+      <c r="C68" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="69" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>566</v>
-      </c>
-      <c r="B69" s="21" t="s">
+        <v>562</v>
+      </c>
+      <c r="B69" s="49"/>
+      <c r="C69" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
+        <v>563</v>
+      </c>
+      <c r="B70" s="49"/>
+      <c r="C70" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="90" t="s">
+        <v>703</v>
+      </c>
+      <c r="B71" s="91"/>
+    </row>
+    <row r="72" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="60" t="s">
+        <v>704</v>
+      </c>
+      <c r="B72" s="61"/>
+    </row>
+    <row r="73" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="62" t="s">
+        <v>705</v>
+      </c>
+      <c r="B73" s="63" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="43" t="s">
-        <v>568</v>
-      </c>
-      <c r="B70" s="44" t="s">
+    <row r="74" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="62" t="s">
+        <v>706</v>
+      </c>
+      <c r="B74" s="63" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
-        <v>570</v>
-      </c>
-      <c r="B71" s="21"/>
-    </row>
-    <row r="72" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20" t="s">
-        <v>571</v>
-      </c>
-      <c r="B72" s="21"/>
-    </row>
-    <row r="73" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
-        <v>572</v>
-      </c>
-      <c r="B73" s="21"/>
-    </row>
-    <row r="74" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="20" t="s">
-        <v>573</v>
-      </c>
-      <c r="B74" s="21"/>
-    </row>
     <row r="75" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="22" t="s">
-        <v>574</v>
-      </c>
-      <c r="B75" s="23"/>
+      <c r="A75" s="62" t="s">
+        <v>707</v>
+      </c>
+      <c r="B75" s="63"/>
     </row>
     <row r="76" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="62" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="62" t="s">
+        <v>709</v>
+      </c>
+      <c r="B77" s="63"/>
+    </row>
+    <row r="78" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="62" t="s">
+        <v>710</v>
+      </c>
+      <c r="B78" s="63"/>
+    </row>
+    <row r="79" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="90" t="s">
+        <v>711</v>
+      </c>
+      <c r="B79" s="91"/>
+    </row>
+    <row r="80" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="60" t="s">
         <v>575</v>
       </c>
-      <c r="B76" s="29" t="s">
+      <c r="B80" s="61" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="s">
+    <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="62" t="s">
         <v>577</v>
       </c>
-      <c r="B77" s="15"/>
-    </row>
-    <row r="78" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
+      <c r="B81" s="63"/>
+    </row>
+    <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="62" t="s">
         <v>578</v>
       </c>
-      <c r="B78" s="15"/>
-    </row>
-    <row r="79" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
+      <c r="B82" s="63"/>
+    </row>
+    <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="60" t="s">
         <v>579</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B83" s="61" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+    <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="64" t="s">
         <v>581</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B84" s="65" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
+    <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="62" t="s">
         <v>582</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B85" s="63" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
+    <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="62" t="s">
         <v>584</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B86" s="63" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="45" t="s">
-        <v>585</v>
-      </c>
-      <c r="B83" s="34"/>
-    </row>
-    <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="24" t="s">
-        <v>586</v>
-      </c>
-      <c r="B84" s="29"/>
-    </row>
-    <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="20" t="s">
-        <v>587</v>
-      </c>
-      <c r="B85" s="15"/>
-    </row>
-    <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="20" t="s">
-        <v>588</v>
-      </c>
-      <c r="B86" s="15"/>
-    </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="22" t="s">
-        <v>589</v>
-      </c>
-      <c r="B87" s="46"/>
+      <c r="A87" s="73" t="s">
+        <v>657</v>
+      </c>
+      <c r="B87" s="74"/>
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="20" t="s">
-        <v>590</v>
-      </c>
-      <c r="B88" s="15"/>
+      <c r="A88" s="60" t="s">
+        <v>658</v>
+      </c>
+      <c r="B88" s="61"/>
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="20" t="s">
-        <v>591</v>
-      </c>
-      <c r="B89" s="15"/>
+      <c r="A89" s="62" t="s">
+        <v>659</v>
+      </c>
+      <c r="B89" s="63"/>
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="20" t="s">
-        <v>592</v>
-      </c>
-      <c r="B90" s="15"/>
+      <c r="A90" s="62" t="s">
+        <v>660</v>
+      </c>
+      <c r="B90" s="63"/>
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="B91" s="46"/>
+      <c r="A91" s="64" t="s">
+        <v>661</v>
+      </c>
+      <c r="B91" s="65"/>
     </row>
     <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="60" t="s">
+        <v>662</v>
+      </c>
+      <c r="B92" s="61"/>
+    </row>
+    <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="62" t="s">
+        <v>663</v>
+      </c>
+      <c r="B93" s="63"/>
+    </row>
+    <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="B94" s="63"/>
+    </row>
+    <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="64" t="s">
+        <v>665</v>
+      </c>
+      <c r="B95" s="65"/>
+    </row>
+    <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="62" t="s">
         <v>594</v>
       </c>
-      <c r="B92" s="29" t="s">
+      <c r="B96" s="63" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="14" t="s">
+    <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="62" t="s">
         <v>596</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B97" s="63" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
+    <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="64" t="s">
         <v>598</v>
       </c>
-      <c r="B94" s="17"/>
-    </row>
-    <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="43" t="s">
-        <v>599</v>
-      </c>
-      <c r="B95" s="44" t="s">
+      <c r="B98" s="65"/>
+    </row>
+    <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="75" t="s">
+        <v>666</v>
+      </c>
+      <c r="B99" s="76" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="43" t="s">
-        <v>601</v>
-      </c>
-      <c r="B96" s="44" t="s">
+    <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="41" t="s">
+        <v>667</v>
+      </c>
+      <c r="B100" s="77" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="43" t="s">
-        <v>603</v>
-      </c>
-      <c r="B97" s="44" t="s">
+    <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="41" t="s">
+        <v>668</v>
+      </c>
+      <c r="B101" s="77" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="43" t="s">
-        <v>605</v>
-      </c>
-      <c r="B98" s="44" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="43" t="s">
-        <v>607</v>
-      </c>
-      <c r="B99" s="44"/>
-    </row>
-    <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="43" t="s">
-        <v>608</v>
-      </c>
-      <c r="B100" s="44"/>
-    </row>
-    <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="47" t="s">
-        <v>609</v>
-      </c>
-      <c r="B101" s="48"/>
-    </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="41" t="s">
+        <v>669</v>
+      </c>
+      <c r="B102" s="77" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="41" t="s">
+        <v>670</v>
+      </c>
+      <c r="B103" s="77"/>
+    </row>
+    <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="41" t="s">
+        <v>671</v>
+      </c>
+      <c r="B104" s="77"/>
+    </row>
+    <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="92" t="s">
+        <v>672</v>
+      </c>
+      <c r="B105" s="93"/>
+    </row>
+    <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="60" t="s">
         <v>610</v>
       </c>
-      <c r="B102" s="29"/>
-    </row>
-    <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14" t="s">
+      <c r="B106" s="61"/>
+    </row>
+    <row r="107" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="62" t="s">
         <v>611</v>
       </c>
-      <c r="B103" s="15"/>
-    </row>
-    <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+      <c r="B107" s="63"/>
+    </row>
+    <row r="108" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="64" t="s">
         <v>612</v>
       </c>
-      <c r="B104" s="17" t="s">
+      <c r="B108" s="65" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="24" t="s">
-        <v>614</v>
-      </c>
-      <c r="B105" s="49"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="50" t="s">
-        <v>615</v>
-      </c>
-      <c r="B106" s="41" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="20" t="s">
-        <v>617</v>
-      </c>
-      <c r="B107" s="51" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="20" t="s">
-        <v>619</v>
-      </c>
-      <c r="B108" s="51" t="s">
-        <v>620</v>
-      </c>
-    </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="50" t="s">
-        <v>621</v>
-      </c>
-      <c r="B109" s="52"/>
-    </row>
-    <row r="110" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
+      <c r="A109" s="60" t="s">
+        <v>673</v>
+      </c>
+      <c r="B109" s="61"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="62" t="s">
+        <v>674</v>
+      </c>
+      <c r="B110" s="79" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="62" t="s">
+        <v>675</v>
+      </c>
+      <c r="B111" s="79" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="62" t="s">
+        <v>676</v>
+      </c>
+      <c r="B112" s="79" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="96" t="s">
+        <v>677</v>
+      </c>
+      <c r="B113" s="97"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="80" t="s">
+        <v>682</v>
+      </c>
+      <c r="B114" s="81"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="78" t="s">
+        <v>681</v>
+      </c>
+      <c r="B115" s="79"/>
+    </row>
+    <row r="116" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="73" t="s">
         <v>622</v>
       </c>
-      <c r="B110" s="26" t="s">
+      <c r="B116" s="74" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="B111" s="26"/>
+    <row r="117" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="60" t="s">
+        <v>678</v>
+      </c>
+      <c r="B117" s="61"/>
+    </row>
+    <row r="118" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="78" t="s">
+        <v>679</v>
+      </c>
+      <c r="B118" s="79"/>
+    </row>
+    <row r="119" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="94" t="s">
+        <v>680</v>
+      </c>
+      <c r="B119" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>